<commit_message>
Guarding Pawns 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/Guarding Pawns - 3114183220/3114183220.xlsx
+++ b/Data/Guarding Pawns - 3114183220/3114183220.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.8.3\Guarding Pawns - 3114183220\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SteamLibrary\steamapps\common\RimWorld\Mods\RMK\Data\Guarding Pawns - 3114183220\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F661108D-CBD7-4966-B353-981569AA2903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53B8177-1C19-46B7-A710-4A5D2D01B226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_240430" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_250701" sheetId="3" r:id="rId1"/>
+    <sheet name="Old_240430" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="344">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -1063,6 +1064,15 @@
   <si>
     <t>폰들이 순찰 지점을 따라 순찰할 때 이동하는 순서입니다. 맨 위에서 시작해 이 목록의 지점을 순서대로 거쳐가게 됩니다.\n\n버튼을 사용해서 각 지점의 순서를 바꿀 수 있으며, 이는 폰들의 순찰 경로를 변경합니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JobDef+GuardingP_AttackMelee.reportString</t>
+  </si>
+  <si>
+    <t>GuardingP_AttackMelee.reportString</t>
+  </si>
+  <si>
+    <t>TargetA 공격 중</t>
   </si>
 </sst>
 </file>
@@ -1416,25 +1426,1614 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F74E3D-FC03-4D23-843B-E894D71E4555}">
+  <dimension ref="A1:F93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="66.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65" style="1" customWidth="1"/>
+    <col min="6" max="6" width="53.85546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="66" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="65" style="1" customWidth="1"/>
-    <col min="6" max="6" width="53.81640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="6" max="6" width="53.85546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1454,7 +3053,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1471,7 +3070,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1488,7 +3087,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1505,7 +3104,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1522,7 +3121,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -1539,7 +3138,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1556,7 +3155,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -1573,7 +3172,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1590,7 +3189,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -1607,7 +3206,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>37</v>
       </c>
@@ -1624,7 +3223,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -1641,7 +3240,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -1658,7 +3257,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -1675,7 +3274,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
@@ -1692,7 +3291,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
@@ -1709,7 +3308,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>55</v>
       </c>
@@ -1726,7 +3325,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
@@ -1743,7 +3342,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
@@ -1760,7 +3359,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>65</v>
       </c>
@@ -1777,7 +3376,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>68</v>
       </c>
@@ -1794,7 +3393,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>71</v>
       </c>
@@ -1811,7 +3410,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
@@ -1828,7 +3427,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>77</v>
       </c>
@@ -1845,7 +3444,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>80</v>
       </c>
@@ -1862,7 +3461,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>83</v>
       </c>
@@ -1879,7 +3478,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>86</v>
       </c>
@@ -1896,7 +3495,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>90</v>
       </c>
@@ -1913,7 +3512,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>93</v>
       </c>
@@ -1930,7 +3529,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>96</v>
       </c>
@@ -1947,7 +3546,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>99</v>
       </c>
@@ -1964,7 +3563,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>101</v>
       </c>
@@ -1981,7 +3580,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>105</v>
       </c>
@@ -1998,7 +3597,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>108</v>
       </c>
@@ -2015,7 +3614,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>110</v>
       </c>
@@ -2032,7 +3631,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>113</v>
       </c>
@@ -2049,7 +3648,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>115</v>
       </c>
@@ -2066,7 +3665,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>118</v>
       </c>
@@ -2083,7 +3682,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>120</v>
       </c>
@@ -2100,7 +3699,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>123</v>
       </c>
@@ -2117,7 +3716,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>125</v>
       </c>
@@ -2134,7 +3733,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>128</v>
       </c>
@@ -2151,7 +3750,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>130</v>
       </c>
@@ -2168,7 +3767,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>133</v>
       </c>
@@ -2185,7 +3784,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>136</v>
       </c>
@@ -2202,7 +3801,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>139</v>
       </c>
@@ -2219,7 +3818,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>141</v>
       </c>
@@ -2236,7 +3835,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>144</v>
       </c>
@@ -2253,7 +3852,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>146</v>
       </c>
@@ -2270,7 +3869,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>149</v>
       </c>
@@ -2287,7 +3886,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>151</v>
       </c>
@@ -2304,7 +3903,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>154</v>
       </c>
@@ -2321,7 +3920,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>156</v>
       </c>
@@ -2338,7 +3937,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>159</v>
       </c>
@@ -2355,7 +3954,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>161</v>
       </c>
@@ -2372,7 +3971,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>164</v>
       </c>
@@ -2389,7 +3988,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>168</v>
       </c>
@@ -2406,7 +4005,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>171</v>
       </c>
@@ -2423,7 +4022,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>174</v>
       </c>
@@ -2440,7 +4039,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>177</v>
       </c>
@@ -2457,7 +4056,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>180</v>
       </c>
@@ -2474,7 +4073,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>183</v>
       </c>
@@ -2491,7 +4090,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>186</v>
       </c>
@@ -2508,7 +4107,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>189</v>
       </c>
@@ -2525,7 +4124,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>192</v>
       </c>
@@ -2542,7 +4141,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>195</v>
       </c>
@@ -2559,7 +4158,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>198</v>
       </c>
@@ -2576,7 +4175,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>201</v>
       </c>
@@ -2593,7 +4192,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>204</v>
       </c>
@@ -2610,7 +4209,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>207</v>
       </c>
@@ -2627,7 +4226,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>210</v>
       </c>
@@ -2644,7 +4243,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>212</v>
       </c>
@@ -2661,7 +4260,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>214</v>
       </c>
@@ -2678,7 +4277,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>216</v>
       </c>
@@ -2695,7 +4294,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>218</v>
       </c>
@@ -2712,7 +4311,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>221</v>
       </c>
@@ -2729,7 +4328,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>224</v>
       </c>
@@ -2746,7 +4345,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>227</v>
       </c>
@@ -2763,7 +4362,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>230</v>
       </c>
@@ -2780,7 +4379,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>233</v>
       </c>
@@ -2797,7 +4396,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>236</v>
       </c>
@@ -2814,7 +4413,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>239</v>
       </c>
@@ -2831,7 +4430,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>242</v>
       </c>
@@ -2848,7 +4447,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>245</v>
       </c>
@@ -2865,7 +4464,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>248</v>
       </c>
@@ -2882,7 +4481,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>251</v>
       </c>
@@ -2899,7 +4498,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>254</v>
       </c>
@@ -2916,7 +4515,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>257</v>
       </c>
@@ -2933,7 +4532,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="68" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6" ht="66" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>260</v>
       </c>
@@ -2950,7 +4549,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>263</v>
       </c>
@@ -2967,7 +4566,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>266</v>
       </c>

</xml_diff>